<commit_message>
Update vehicle list: Replace with 4 specific vehicles
</commit_message>
<xml_diff>
--- a/form_data.xlsx
+++ b/form_data.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vehicles" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FuelLevels" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ExteriorChecks" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EngineChecks" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SafetyEquipment" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="InteriorChecks" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Items" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Vehicles" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="FuelLevels" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ExteriorChecks" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="EngineChecks" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="SafetyEquipment" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="InteriorChecks" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Items" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Users" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,21 +438,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SPRINTER: BT-48331</t>
+          <t>SPRINTER: BT-48331 ; RAM-Promaster 2500 (2021)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RAM-Promaster 2500 (2021)</t>
+          <t>SPRINTER: BV-14827 ; MERCEDES- 2500 Cargo Van (2013)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MERCEDES-2500 Cargo Van (2013)</t>
+          <t>SPRINTER: CA-30264 ; MERCEDES-2500 Cargo Van (2024)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TRUCK: CD-53631 ; ISUZU- NRR (2019)</t>
         </is>
       </c>
     </row>

</xml_diff>